<commit_message>
Changed position of legend in plot
Added data for Uppsala.
Moved the legend to always be in the upper right corner, outside of the plot.
</commit_message>
<xml_diff>
--- a/svensk_ mäklarstatistik_bostadsrätter_streamlit.xlsx
+++ b/svensk_ mäklarstatistik_bostadsrätter_streamlit.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="41">
   <si>
     <t xml:space="preserve">År</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t xml:space="preserve">Västerås</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uppsala</t>
   </si>
 </sst>
 </file>
@@ -149,7 +152,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -171,12 +174,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -230,7 +227,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -423,10 +420,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C233"/>
+  <dimension ref="A1:C262"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A193" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F234" activeCellId="0" sqref="F234"/>
+      <selection pane="topLeft" activeCell="E230" activeCellId="0" sqref="E230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2042,10 +2039,10 @@
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="0" t="s">
+      <c r="A147" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B147" s="0" t="n">
+      <c r="B147" s="1" t="n">
         <v>3373</v>
       </c>
       <c r="C147" s="2" t="s">
@@ -2053,10 +2050,10 @@
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="0" t="s">
+      <c r="A148" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B148" s="0" t="n">
+      <c r="B148" s="1" t="n">
         <v>4081</v>
       </c>
       <c r="C148" s="2" t="s">
@@ -2064,10 +2061,10 @@
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="0" t="s">
+      <c r="A149" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B149" s="0" t="n">
+      <c r="B149" s="1" t="n">
         <v>4695</v>
       </c>
       <c r="C149" s="2" t="s">
@@ -2075,10 +2072,10 @@
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="0" t="s">
+      <c r="A150" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B150" s="0" t="n">
+      <c r="B150" s="1" t="n">
         <v>6592</v>
       </c>
       <c r="C150" s="2" t="s">
@@ -2086,10 +2083,10 @@
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="0" t="s">
+      <c r="A151" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B151" s="0" t="n">
+      <c r="B151" s="1" t="n">
         <v>8456</v>
       </c>
       <c r="C151" s="2" t="s">
@@ -2097,10 +2094,10 @@
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="0" t="s">
+      <c r="A152" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B152" s="0" t="n">
+      <c r="B152" s="1" t="n">
         <v>9591</v>
       </c>
       <c r="C152" s="2" t="s">
@@ -2108,10 +2105,10 @@
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="0" t="s">
+      <c r="A153" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B153" s="0" t="n">
+      <c r="B153" s="1" t="n">
         <v>11010</v>
       </c>
       <c r="C153" s="2" t="s">
@@ -2119,10 +2116,10 @@
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="0" t="s">
+      <c r="A154" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B154" s="0" t="n">
+      <c r="B154" s="1" t="n">
         <v>13148</v>
       </c>
       <c r="C154" s="2" t="s">
@@ -2130,10 +2127,10 @@
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="0" t="s">
+      <c r="A155" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B155" s="0" t="n">
+      <c r="B155" s="1" t="n">
         <v>15452</v>
       </c>
       <c r="C155" s="2" t="s">
@@ -2141,10 +2138,10 @@
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="0" t="s">
+      <c r="A156" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B156" s="0" t="n">
+      <c r="B156" s="1" t="n">
         <v>18128</v>
       </c>
       <c r="C156" s="2" t="s">
@@ -2152,10 +2149,10 @@
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="0" t="s">
+      <c r="A157" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B157" s="0" t="n">
+      <c r="B157" s="1" t="n">
         <v>21194</v>
       </c>
       <c r="C157" s="2" t="s">
@@ -2163,10 +2160,10 @@
       </c>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="0" t="s">
+      <c r="A158" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B158" s="0" t="n">
+      <c r="B158" s="1" t="n">
         <v>23133</v>
       </c>
       <c r="C158" s="2" t="s">
@@ -2174,10 +2171,10 @@
       </c>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="0" t="s">
+      <c r="A159" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B159" s="0" t="n">
+      <c r="B159" s="1" t="n">
         <v>22514</v>
       </c>
       <c r="C159" s="2" t="s">
@@ -2185,10 +2182,10 @@
       </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="0" t="s">
+      <c r="A160" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B160" s="0" t="n">
+      <c r="B160" s="1" t="n">
         <v>23542</v>
       </c>
       <c r="C160" s="2" t="s">
@@ -2196,10 +2193,10 @@
       </c>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="0" t="s">
+      <c r="A161" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B161" s="0" t="n">
+      <c r="B161" s="1" t="n">
         <v>26032</v>
       </c>
       <c r="C161" s="2" t="s">
@@ -2207,10 +2204,10 @@
       </c>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="0" t="s">
+      <c r="A162" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B162" s="0" t="n">
+      <c r="B162" s="1" t="n">
         <v>26444</v>
       </c>
       <c r="C162" s="2" t="s">
@@ -2218,10 +2215,10 @@
       </c>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="0" t="s">
+      <c r="A163" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B163" s="0" t="n">
+      <c r="B163" s="1" t="n">
         <v>27816</v>
       </c>
       <c r="C163" s="2" t="s">
@@ -2229,10 +2226,10 @@
       </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="0" t="s">
+      <c r="A164" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B164" s="0" t="n">
+      <c r="B164" s="1" t="n">
         <v>30789</v>
       </c>
       <c r="C164" s="2" t="s">
@@ -2240,10 +2237,10 @@
       </c>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="0" t="s">
+      <c r="A165" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B165" s="0" t="n">
+      <c r="B165" s="1" t="n">
         <v>33366</v>
       </c>
       <c r="C165" s="2" t="s">
@@ -2251,10 +2248,10 @@
       </c>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="0" t="s">
+      <c r="A166" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B166" s="0" t="n">
+      <c r="B166" s="1" t="n">
         <v>40296</v>
       </c>
       <c r="C166" s="2" t="s">
@@ -2262,10 +2259,10 @@
       </c>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="0" t="s">
+      <c r="A167" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B167" s="0" t="n">
+      <c r="B167" s="1" t="n">
         <v>44430</v>
       </c>
       <c r="C167" s="2" t="s">
@@ -2273,10 +2270,10 @@
       </c>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="0" t="s">
+      <c r="A168" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B168" s="0" t="n">
+      <c r="B168" s="1" t="n">
         <v>48865</v>
       </c>
       <c r="C168" s="2" t="s">
@@ -2284,10 +2281,10 @@
       </c>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="0" t="s">
+      <c r="A169" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B169" s="0" t="n">
+      <c r="B169" s="1" t="n">
         <v>47207</v>
       </c>
       <c r="C169" s="2" t="s">
@@ -2295,10 +2292,10 @@
       </c>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="0" t="s">
+      <c r="A170" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B170" s="0" t="n">
+      <c r="B170" s="1" t="n">
         <v>47685</v>
       </c>
       <c r="C170" s="2" t="s">
@@ -2306,10 +2303,10 @@
       </c>
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="0" t="s">
+      <c r="A171" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B171" s="0" t="n">
+      <c r="B171" s="1" t="n">
         <v>49632</v>
       </c>
       <c r="C171" s="2" t="s">
@@ -2317,10 +2314,10 @@
       </c>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="0" t="s">
+      <c r="A172" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B172" s="0" t="n">
+      <c r="B172" s="1" t="n">
         <v>52764</v>
       </c>
       <c r="C172" s="2" t="s">
@@ -2328,10 +2325,10 @@
       </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="0" t="s">
+      <c r="A173" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B173" s="0" t="n">
+      <c r="B173" s="1" t="n">
         <v>52215</v>
       </c>
       <c r="C173" s="2" t="s">
@@ -2339,10 +2336,10 @@
       </c>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="0" t="s">
+      <c r="A174" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B174" s="0" t="n">
+      <c r="B174" s="1" t="n">
         <v>49466</v>
       </c>
       <c r="C174" s="2" t="s">
@@ -2350,10 +2347,10 @@
       </c>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="0" t="s">
+      <c r="A175" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B175" s="0" t="n">
+      <c r="B175" s="1" t="n">
         <v>50249</v>
       </c>
       <c r="C175" s="2" t="s">
@@ -2361,10 +2358,10 @@
       </c>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="0" t="s">
+      <c r="A176" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B176" s="0" t="n">
+      <c r="B176" s="1" t="n">
         <v>1763</v>
       </c>
       <c r="C176" s="2" t="s">
@@ -2372,10 +2369,10 @@
       </c>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="0" t="s">
+      <c r="A177" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B177" s="0" t="n">
+      <c r="B177" s="1" t="n">
         <v>1659</v>
       </c>
       <c r="C177" s="2" t="s">
@@ -2383,10 +2380,10 @@
       </c>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="0" t="s">
+      <c r="A178" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B178" s="0" t="n">
+      <c r="B178" s="1" t="n">
         <v>1945</v>
       </c>
       <c r="C178" s="2" t="s">
@@ -2394,10 +2391,10 @@
       </c>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="0" t="s">
+      <c r="A179" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B179" s="0" t="n">
+      <c r="B179" s="1" t="n">
         <v>1850</v>
       </c>
       <c r="C179" s="2" t="s">
@@ -2405,10 +2402,10 @@
       </c>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="0" t="s">
+      <c r="A180" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B180" s="0" t="n">
+      <c r="B180" s="1" t="n">
         <v>2256</v>
       </c>
       <c r="C180" s="2" t="s">
@@ -2416,10 +2413,10 @@
       </c>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="0" t="s">
+      <c r="A181" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B181" s="0" t="n">
+      <c r="B181" s="1" t="n">
         <v>2294</v>
       </c>
       <c r="C181" s="2" t="s">
@@ -2427,10 +2424,10 @@
       </c>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="0" t="s">
+      <c r="A182" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B182" s="0" t="n">
+      <c r="B182" s="1" t="n">
         <v>2401</v>
       </c>
       <c r="C182" s="2" t="s">
@@ -2438,10 +2435,10 @@
       </c>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="0" t="s">
+      <c r="A183" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B183" s="0" t="n">
+      <c r="B183" s="1" t="n">
         <v>3027</v>
       </c>
       <c r="C183" s="2" t="s">
@@ -2449,10 +2446,10 @@
       </c>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="0" t="s">
+      <c r="A184" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B184" s="0" t="n">
+      <c r="B184" s="1" t="n">
         <v>4065</v>
       </c>
       <c r="C184" s="2" t="s">
@@ -2460,10 +2457,10 @@
       </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="0" t="s">
+      <c r="A185" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B185" s="0" t="n">
+      <c r="B185" s="1" t="n">
         <v>4745</v>
       </c>
       <c r="C185" s="2" t="s">
@@ -2471,10 +2468,10 @@
       </c>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="0" t="s">
+      <c r="A186" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B186" s="0" t="n">
+      <c r="B186" s="1" t="n">
         <v>5683</v>
       </c>
       <c r="C186" s="2" t="s">
@@ -2482,10 +2479,10 @@
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="0" t="s">
+      <c r="A187" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B187" s="0" t="n">
+      <c r="B187" s="1" t="n">
         <v>7168</v>
       </c>
       <c r="C187" s="2" t="s">
@@ -2493,10 +2490,10 @@
       </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="0" t="s">
+      <c r="A188" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B188" s="0" t="n">
+      <c r="B188" s="1" t="n">
         <v>7719</v>
       </c>
       <c r="C188" s="2" t="s">
@@ -2504,10 +2501,10 @@
       </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="0" t="s">
+      <c r="A189" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B189" s="0" t="n">
+      <c r="B189" s="1" t="n">
         <v>9712</v>
       </c>
       <c r="C189" s="2" t="s">
@@ -2515,10 +2512,10 @@
       </c>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="0" t="s">
+      <c r="A190" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B190" s="0" t="n">
+      <c r="B190" s="1" t="n">
         <v>10193</v>
       </c>
       <c r="C190" s="2" t="s">
@@ -2526,10 +2523,10 @@
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="0" t="s">
+      <c r="A191" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B191" s="0" t="n">
+      <c r="B191" s="1" t="n">
         <v>10818</v>
       </c>
       <c r="C191" s="2" t="s">
@@ -2537,10 +2534,10 @@
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="0" t="s">
+      <c r="A192" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B192" s="0" t="n">
+      <c r="B192" s="1" t="n">
         <v>11621</v>
       </c>
       <c r="C192" s="2" t="s">
@@ -2548,10 +2545,10 @@
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="0" t="s">
+      <c r="A193" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B193" s="0" t="n">
+      <c r="B193" s="1" t="n">
         <v>13297</v>
       </c>
       <c r="C193" s="2" t="s">
@@ -2559,10 +2556,10 @@
       </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="0" t="s">
+      <c r="A194" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B194" s="0" t="n">
+      <c r="B194" s="1" t="n">
         <v>16627</v>
       </c>
       <c r="C194" s="2" t="s">
@@ -2570,10 +2567,10 @@
       </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="0" t="s">
+      <c r="A195" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B195" s="0" t="n">
+      <c r="B195" s="1" t="n">
         <v>19039</v>
       </c>
       <c r="C195" s="2" t="s">
@@ -2581,10 +2578,10 @@
       </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="0" t="s">
+      <c r="A196" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B196" s="0" t="n">
+      <c r="B196" s="1" t="n">
         <v>21819</v>
       </c>
       <c r="C196" s="2" t="s">
@@ -2592,10 +2589,10 @@
       </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="0" t="s">
+      <c r="A197" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B197" s="0" t="n">
+      <c r="B197" s="1" t="n">
         <v>24769</v>
       </c>
       <c r="C197" s="2" t="s">
@@ -2603,10 +2600,10 @@
       </c>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="0" t="s">
+      <c r="A198" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B198" s="0" t="n">
+      <c r="B198" s="1" t="n">
         <v>24167</v>
       </c>
       <c r="C198" s="2" t="s">
@@ -2614,10 +2611,10 @@
       </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="0" t="s">
+      <c r="A199" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B199" s="0" t="n">
+      <c r="B199" s="1" t="n">
         <v>25000</v>
       </c>
       <c r="C199" s="2" t="s">
@@ -2625,10 +2622,10 @@
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="0" t="s">
+      <c r="A200" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B200" s="0" t="n">
+      <c r="B200" s="1" t="n">
         <v>26387</v>
       </c>
       <c r="C200" s="2" t="s">
@@ -2636,10 +2633,10 @@
       </c>
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="0" t="s">
+      <c r="A201" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B201" s="0" t="n">
+      <c r="B201" s="1" t="n">
         <v>28193</v>
       </c>
       <c r="C201" s="2" t="s">
@@ -2647,10 +2644,10 @@
       </c>
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="0" t="s">
+      <c r="A202" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B202" s="0" t="n">
+      <c r="B202" s="1" t="n">
         <v>27705</v>
       </c>
       <c r="C202" s="2" t="s">
@@ -2658,10 +2655,10 @@
       </c>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="0" t="s">
+      <c r="A203" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B203" s="0" t="n">
+      <c r="B203" s="1" t="n">
         <v>25662</v>
       </c>
       <c r="C203" s="2" t="s">
@@ -2669,10 +2666,10 @@
       </c>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="0" t="s">
+      <c r="A204" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B204" s="0" t="n">
+      <c r="B204" s="1" t="n">
         <v>25717</v>
       </c>
       <c r="C204" s="2" t="s">
@@ -2680,10 +2677,10 @@
       </c>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="0" t="s">
+      <c r="A205" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B205" s="0" t="n">
+      <c r="B205" s="1" t="n">
         <v>1867</v>
       </c>
       <c r="C205" s="2" t="s">
@@ -2691,10 +2688,10 @@
       </c>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="0" t="s">
+      <c r="A206" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B206" s="0" t="n">
+      <c r="B206" s="1" t="n">
         <v>2249</v>
       </c>
       <c r="C206" s="2" t="s">
@@ -2702,10 +2699,10 @@
       </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="0" t="s">
+      <c r="A207" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B207" s="0" t="n">
+      <c r="B207" s="1" t="n">
         <v>2353</v>
       </c>
       <c r="C207" s="2" t="s">
@@ -2713,10 +2710,10 @@
       </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="0" t="s">
+      <c r="A208" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B208" s="0" t="n">
+      <c r="B208" s="1" t="n">
         <v>2752</v>
       </c>
       <c r="C208" s="2" t="s">
@@ -2724,10 +2721,10 @@
       </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="0" t="s">
+      <c r="A209" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B209" s="0" t="n">
+      <c r="B209" s="1" t="n">
         <v>2282</v>
       </c>
       <c r="C209" s="2" t="s">
@@ -2735,10 +2732,10 @@
       </c>
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="0" t="s">
+      <c r="A210" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B210" s="0" t="n">
+      <c r="B210" s="1" t="n">
         <v>2993</v>
       </c>
       <c r="C210" s="2" t="s">
@@ -2746,10 +2743,10 @@
       </c>
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="0" t="s">
+      <c r="A211" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B211" s="0" t="n">
+      <c r="B211" s="1" t="n">
         <v>4035</v>
       </c>
       <c r="C211" s="2" t="s">
@@ -2757,10 +2754,10 @@
       </c>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="0" t="s">
+      <c r="A212" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B212" s="0" t="n">
+      <c r="B212" s="1" t="n">
         <v>4288</v>
       </c>
       <c r="C212" s="2" t="s">
@@ -2768,10 +2765,10 @@
       </c>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="0" t="s">
+      <c r="A213" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B213" s="0" t="n">
+      <c r="B213" s="1" t="n">
         <v>5573</v>
       </c>
       <c r="C213" s="2" t="s">
@@ -2779,10 +2776,10 @@
       </c>
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="0" t="s">
+      <c r="A214" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B214" s="0" t="n">
+      <c r="B214" s="1" t="n">
         <v>6930</v>
       </c>
       <c r="C214" s="2" t="s">
@@ -2790,10 +2787,10 @@
       </c>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="0" t="s">
+      <c r="A215" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B215" s="0" t="n">
+      <c r="B215" s="1" t="n">
         <v>8355</v>
       </c>
       <c r="C215" s="2" t="s">
@@ -2801,10 +2798,10 @@
       </c>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="0" t="s">
+      <c r="A216" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B216" s="0" t="n">
+      <c r="B216" s="1" t="n">
         <v>10220</v>
       </c>
       <c r="C216" s="2" t="s">
@@ -2812,10 +2809,10 @@
       </c>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="0" t="s">
+      <c r="A217" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B217" s="0" t="n">
+      <c r="B217" s="1" t="n">
         <v>10526</v>
       </c>
       <c r="C217" s="2" t="s">
@@ -2823,10 +2820,10 @@
       </c>
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="0" t="s">
+      <c r="A218" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B218" s="0" t="n">
+      <c r="B218" s="1" t="n">
         <v>12032</v>
       </c>
       <c r="C218" s="2" t="s">
@@ -2834,10 +2831,10 @@
       </c>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="0" t="s">
+      <c r="A219" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B219" s="0" t="n">
+      <c r="B219" s="1" t="n">
         <v>11874</v>
       </c>
       <c r="C219" s="2" t="s">
@@ -2845,10 +2842,10 @@
       </c>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="0" t="s">
+      <c r="A220" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B220" s="0" t="n">
+      <c r="B220" s="1" t="n">
         <v>11394</v>
       </c>
       <c r="C220" s="2" t="s">
@@ -2856,10 +2853,10 @@
       </c>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="0" t="s">
+      <c r="A221" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B221" s="0" t="n">
+      <c r="B221" s="1" t="n">
         <v>12010</v>
       </c>
       <c r="C221" s="2" t="s">
@@ -2867,10 +2864,10 @@
       </c>
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A222" s="0" t="s">
+      <c r="A222" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B222" s="0" t="n">
+      <c r="B222" s="1" t="n">
         <v>13208</v>
       </c>
       <c r="C222" s="2" t="s">
@@ -2878,10 +2875,10 @@
       </c>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="0" t="s">
+      <c r="A223" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B223" s="0" t="n">
+      <c r="B223" s="1" t="n">
         <v>14852</v>
       </c>
       <c r="C223" s="2" t="s">
@@ -2889,10 +2886,10 @@
       </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="0" t="s">
+      <c r="A224" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B224" s="0" t="n">
+      <c r="B224" s="1" t="n">
         <v>17806</v>
       </c>
       <c r="C224" s="2" t="s">
@@ -2900,10 +2897,10 @@
       </c>
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="0" t="s">
+      <c r="A225" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B225" s="0" t="n">
+      <c r="B225" s="1" t="n">
         <v>20244</v>
       </c>
       <c r="C225" s="2" t="s">
@@ -2911,10 +2908,10 @@
       </c>
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="0" t="s">
+      <c r="A226" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B226" s="0" t="n">
+      <c r="B226" s="1" t="n">
         <v>22426</v>
       </c>
       <c r="C226" s="2" t="s">
@@ -2922,10 +2919,10 @@
       </c>
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="0" t="s">
+      <c r="A227" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B227" s="0" t="n">
+      <c r="B227" s="1" t="n">
         <v>22225</v>
       </c>
       <c r="C227" s="2" t="s">
@@ -2933,10 +2930,10 @@
       </c>
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="0" t="s">
+      <c r="A228" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B228" s="0" t="n">
+      <c r="B228" s="1" t="n">
         <v>22792</v>
       </c>
       <c r="C228" s="2" t="s">
@@ -2944,10 +2941,10 @@
       </c>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="0" t="s">
+      <c r="A229" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B229" s="0" t="n">
+      <c r="B229" s="1" t="n">
         <v>23838</v>
       </c>
       <c r="C229" s="2" t="s">
@@ -2955,10 +2952,10 @@
       </c>
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="0" t="s">
+      <c r="A230" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B230" s="0" t="n">
+      <c r="B230" s="1" t="n">
         <v>26283</v>
       </c>
       <c r="C230" s="2" t="s">
@@ -2966,10 +2963,10 @@
       </c>
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="0" t="s">
+      <c r="A231" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B231" s="0" t="n">
+      <c r="B231" s="1" t="n">
         <v>25645</v>
       </c>
       <c r="C231" s="2" t="s">
@@ -2977,10 +2974,10 @@
       </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="0" t="s">
+      <c r="A232" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B232" s="0" t="n">
+      <c r="B232" s="1" t="n">
         <v>23873</v>
       </c>
       <c r="C232" s="2" t="s">
@@ -2988,14 +2985,333 @@
       </c>
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="0" t="s">
+      <c r="A233" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B233" s="0" t="n">
+      <c r="B233" s="1" t="n">
         <v>24003</v>
       </c>
       <c r="C233" s="2" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B234" s="0" t="n">
+        <v>4036</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B235" s="0" t="n">
+        <v>4566</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B236" s="0" t="n">
+        <v>5614</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B237" s="0" t="n">
+        <v>6743</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B238" s="0" t="n">
+        <v>8496</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B239" s="0" t="n">
+        <v>9647</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B240" s="0" t="n">
+        <v>11459</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B241" s="0" t="n">
+        <v>12145</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B242" s="0" t="n">
+        <v>13589</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B243" s="0" t="n">
+        <v>14737</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B244" s="0" t="n">
+        <v>15640</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B245" s="0" t="n">
+        <v>17936</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B246" s="0" t="n">
+        <v>18377</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B247" s="0" t="n">
+        <v>20350</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B248" s="0" t="n">
+        <v>23963</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B249" s="0" t="n">
+        <v>25773</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B250" s="0" t="n">
+        <v>27295</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B251" s="0" t="n">
+        <v>30135</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A252" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B252" s="0" t="n">
+        <v>34332</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A253" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B253" s="0" t="n">
+        <v>37695</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B254" s="0" t="n">
+        <v>39007</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B255" s="0" t="n">
+        <v>40307</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B256" s="0" t="n">
+        <v>37120</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B257" s="0" t="n">
+        <v>37762</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B258" s="0" t="n">
+        <v>39399</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B259" s="0" t="n">
+        <v>42762</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B260" s="0" t="n">
+        <v>42336</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B261" s="0" t="n">
+        <v>40020</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B262" s="0" t="n">
+        <v>40193</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>